<commit_message>
Adding latest model version
</commit_message>
<xml_diff>
--- a/PIT-Parameters.xlsx
+++ b/PIT-Parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldbankgroup-my.sharepoint.com/personal/jsimonov_worldbank_org/Documents/Documents/WB/Countries/Moldova/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="358" documentId="8_{F7A9F20A-4427-4DF5-9138-8D91B718E85D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0CD03BD7-0F36-4137-87DC-503B11299653}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="13_ncr:1_{55716DA5-BCB8-4E08-9BA0-37E92AF8CC69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C6585CB-D80D-4675-9002-96D6712A500D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D2CE6FB8-BE68-4D02-9EDD-4716A6CE79A3}"/>
   </bookViews>
@@ -36,50 +36,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="163">
-  <si>
-    <t>rate1</t>
-  </si>
-  <si>
-    <t>rate2</t>
-  </si>
-  <si>
-    <t>rate3</t>
-  </si>
-  <si>
-    <t>rate4</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="185">
   <si>
     <t>Descriptions</t>
   </si>
   <si>
-    <t>PIT tax rate 1</t>
-  </si>
-  <si>
-    <t>PIT tax rate 2</t>
-  </si>
-  <si>
-    <t>PIT tax rate 3</t>
-  </si>
-  <si>
-    <t>PIT tax rate 4</t>
-  </si>
-  <si>
     <t>LongName</t>
   </si>
   <si>
-    <t>The lowest tax rate, applied to the portion of taxable income below tax bracket 1</t>
-  </si>
-  <si>
-    <t>Tax rate applied to gross income higher than bracket 1 and lower than bracket 2</t>
-  </si>
-  <si>
-    <t>Tax rate applied to gross income higher than bracket 2 and lower than bracket 3</t>
-  </si>
-  <si>
-    <t>Tax rate applied to gross income higher than bracket 4</t>
-  </si>
-  <si>
     <t>Parameters</t>
   </si>
   <si>
@@ -101,9 +65,6 @@
     <t>Deductions</t>
   </si>
   <si>
-    <t>Article 11(1) of LAW ON PERSONAL INCOME TAX. Tax on income from gains from all types of incomes (expect games of chance) be paid at a single 10% rate.</t>
-  </si>
-  <si>
     <t>Variables</t>
   </si>
   <si>
@@ -179,9 +140,6 @@
     <t>var27</t>
   </si>
   <si>
-    <t xml:space="preserve">Progressive Rate </t>
-  </si>
-  <si>
     <t>rate_indiv_art15a</t>
   </si>
   <si>
@@ -246,60 +204,6 @@
   </si>
   <si>
     <t>ded_cash_m_art69_11</t>
-  </si>
-  <si>
-    <r>
-      <t>Article 69</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">11, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Tax rate, par 1-The income tax rate represents 1% of the object of taxation, but not less than
-MDL 3 000</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Article 69</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>11</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,  Tax rate, par 2-In the first tax period, the taxpayer is entitled to diminish the due income tax amount with the expenses amount incurred for the purchase (acquirement) of the cash
-register equipment used in the activity</t>
-    </r>
   </si>
   <si>
     <t>The natural person who carries out independent activity 
@@ -500,9 +404,6 @@
     <t>​In 2023, the fixed annual mandatory health insurance premium in Moldova was 12,636 MDL</t>
   </si>
   <si>
-    <t>Article 69 (TAX REGIME OF THE NATURAL PERSONS CARRYING OUT ACTIVITIES INTHE FIELD OF PURCHASES OF CROP AND/OR HORTICULTURAL PRODUCTS AND/OR VEGETABLE KINGDOM OBJECTS)</t>
-  </si>
-  <si>
     <t>Article 71. Non-residents' income received in the Republic of Moldova - Other payments directed to the non-resident related to income from art. 71, except for dividends and the amounts specified in art. 901 paragraph (31) third indent of the Tax Code</t>
   </si>
   <si>
@@ -578,6 +479,109 @@
     <t>var38</t>
   </si>
   <si>
+    <t>var5</t>
+  </si>
+  <si>
+    <t>Article 69¹¹,  Tax rate, par 2-In the first tax period, the taxpayer is entitled to diminish the due income tax amount with the expenses amount incurred for the purchase (acquirement) of the cash
+register equipment used in the activity</t>
+  </si>
+  <si>
+    <t>Article 69¹¹ Tax rate, par 1-The income tax rate represents 1% of the object of taxation, but not less than
+MDL 3 000 (rate)</t>
+  </si>
+  <si>
+    <t>Article 69¹¹ Tax rate, par 1-The income tax rate represents 1% of the object of taxation, but not less than
+MDL 3 000 (fixed amount)</t>
+  </si>
+  <si>
+    <t>Tax rate applied to gross income higher than bracket 1 and lower than bracket 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Progressive Rate </t>
+  </si>
+  <si>
+    <t>PIT tax rate 2</t>
+  </si>
+  <si>
+    <t>rate2</t>
+  </si>
+  <si>
+    <t>Tax rate applied to gross income higher than bracket 2 and lower than bracket 3</t>
+  </si>
+  <si>
+    <t>PIT tax rate 3</t>
+  </si>
+  <si>
+    <t>rate3</t>
+  </si>
+  <si>
+    <t>Tax rate applied to gross income higher than bracket 4</t>
+  </si>
+  <si>
+    <t>PIT tax rate 4</t>
+  </si>
+  <si>
+    <t>rate4</t>
+  </si>
+  <si>
+    <t>Tax Brackets</t>
+  </si>
+  <si>
+    <t>Gross Incomes smaller than Threshold 1 are taxed at Tax Rate 1</t>
+  </si>
+  <si>
+    <t>Simulation1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PIT tax bracket 1 </t>
+  </si>
+  <si>
+    <t>tbrk1</t>
+  </si>
+  <si>
+    <t>Gross Incomes greater than Threshold 1 and smaller than Threshold 3 are taxed at Tax Rate 2</t>
+  </si>
+  <si>
+    <t>Simulation2</t>
+  </si>
+  <si>
+    <t>PIT tax bracket 2</t>
+  </si>
+  <si>
+    <t>tbrk2</t>
+  </si>
+  <si>
+    <t>Gross Incomes greater than Threshold 1 and smaller than Threshold 2 are taxed at Tax Rate 3</t>
+  </si>
+  <si>
+    <t>Simulation3</t>
+  </si>
+  <si>
+    <t>PIT tax bracket 3</t>
+  </si>
+  <si>
+    <t>tbrk3</t>
+  </si>
+  <si>
+    <t>Gross Incomes greater than Threshold 1 and smaller than Threshold 2 are taxed at Tax Rate 4</t>
+  </si>
+  <si>
+    <t>Simulation4</t>
+  </si>
+  <si>
+    <t>PIT tax bracket 4</t>
+  </si>
+  <si>
+    <t>tbrk4</t>
+  </si>
+  <si>
+    <t>Article 69¹⁷ (The object of taxation is the income from the sale of the crop and/or horticulture
+products and/or vegetal kingdom objects to the economic agent.)</t>
+  </si>
+  <si>
+    <t>Income exempt from prior withholding of income tax according to art. 90 from the Tax Code</t>
+  </si>
+  <si>
     <t>var39</t>
   </si>
   <si>
@@ -591,13 +595,31 @@
   </si>
   <si>
     <t>var43</t>
+  </si>
+  <si>
+    <t>var44</t>
+  </si>
+  <si>
+    <t>var45</t>
+  </si>
+  <si>
+    <t>Toggles</t>
+  </si>
+  <si>
+    <t>var46</t>
+  </si>
+  <si>
+    <t>Introducing Progression All incomes</t>
+  </si>
+  <si>
+    <t>toggle_progression_all</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -615,21 +637,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="4"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -670,7 +677,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -678,10 +685,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1000,10 +1004,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91E408EA-5866-401D-ACA9-2C1AFA6CBF44}">
-  <dimension ref="A1:H70"/>
+  <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="E41" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P45" sqref="P45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,1107 +1024,1199 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="E1" s="4" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="3">
+        <v>2023</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E3" s="3">
+        <v>2023</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E4" s="3">
+        <v>2023</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2023</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="3">
+        <v>2023</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="5">
-        <v>2023</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="6">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" s="5">
-        <v>2023</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" s="6">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="5">
-        <v>2023</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" s="6">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" s="5">
-        <v>2023</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="H5" s="6">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="32.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E6" s="3">
-        <v>2023</v>
-      </c>
-      <c r="F6" s="2" t="s">
+      <c r="D7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2023</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="H6" s="2">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="32.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E7" s="3">
-        <v>2023</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="H7" s="2">
-        <v>3000</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>81</v>
+        <v>143</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>145</v>
+        <v>15</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>82</v>
+        <v>56</v>
       </c>
       <c r="E8" s="3">
         <v>2023</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="H8" s="2">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>85</v>
+        <v>144</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="E9" s="3">
         <v>2023</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="H9" s="2">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>84</v>
+        <v>111</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>29</v>
+        <v>129</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="E10" s="3">
         <v>2023</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="H10" s="2">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>127</v>
+        <v>172</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>122</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D11" s="3"/>
       <c r="E11" s="3">
         <v>2023</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>123</v>
+        <v>40</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>123</v>
+        <v>40</v>
       </c>
       <c r="H11" s="2">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3">
         <v>2023</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="H12" s="2">
-        <v>0.06</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3">
         <v>2023</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="H13" s="2">
         <v>0.12</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3">
         <v>2023</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="H14" s="2">
         <v>0.12</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3">
         <v>2023</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="H15" s="2">
         <v>0.12</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3">
         <v>2023</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="H16" s="2">
         <v>0.12</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3">
         <v>2023</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="H17" s="2">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3">
         <v>2023</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="H18" s="2">
         <v>0.06</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3">
         <v>2023</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="H19" s="2">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3">
         <v>2023</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="H20" s="2">
-        <v>0.18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3">
         <v>2023</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="H21" s="2">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>19</v>
+        <v>155</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D22" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>157</v>
+      </c>
       <c r="E22" s="3">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>64</v>
+        <v>158</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>64</v>
+        <v>159</v>
       </c>
       <c r="H22" s="2">
-        <v>0.12</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>19</v>
+        <v>155</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>143</v>
+        <v>160</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D23" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>161</v>
+      </c>
       <c r="E23" s="3">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>65</v>
+        <v>162</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>65</v>
+        <v>163</v>
       </c>
       <c r="H23" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>124</v>
+        <v>155</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>130</v>
+        <v>164</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="E24" s="3">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>125</v>
+        <v>166</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>125</v>
+        <v>167</v>
       </c>
       <c r="H24" s="2">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="E25" s="3">
+        <v>2021</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="H25" s="2">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E26" s="3">
+        <v>2023</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H26" s="2">
         <v>14700</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="E25" s="3">
-        <v>2023</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="H25" s="2">
+    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E27" s="3">
+        <v>2023</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="H27" s="2">
         <v>12636</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3">
-        <v>2023</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H26" s="2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3">
+        <v>2023</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H28" s="2">
         <v>0.09</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E27" s="3">
-        <v>2023</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H27" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E28" s="3">
-        <v>2023</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="H28" s="2">
-        <v>0.05</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>76</v>
+        <v>142</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="E29" s="3">
         <v>2023</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="H29" s="2">
-        <v>2E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>86</v>
+        <v>59</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>87</v>
+        <v>61</v>
       </c>
       <c r="E30" s="3">
         <v>2023</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="H30" s="2">
-        <v>27000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="210" x14ac:dyDescent="0.25">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>92</v>
+        <v>60</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="E31" s="3">
         <v>2023</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="H31" s="2">
-        <v>31500</v>
+        <v>2E-3</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="E32" s="3">
         <v>2023</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="H32" s="2">
-        <v>19800</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>27000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="210" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="E33" s="3">
         <v>2023</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="H33" s="2">
-        <v>9000</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>31500</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="E34" s="3">
         <v>2023</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="H34" s="2">
         <v>19800</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>121</v>
+        <v>8</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>113</v>
+        <v>74</v>
       </c>
       <c r="E35" s="3">
         <v>2023</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>103</v>
+        <v>38</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>103</v>
+        <v>38</v>
       </c>
       <c r="H35" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>121</v>
+        <v>8</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>105</v>
+        <v>78</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>114</v>
+        <v>75</v>
       </c>
       <c r="E36" s="3">
         <v>2023</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>95</v>
+        <v>39</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>95</v>
+        <v>39</v>
       </c>
       <c r="H36" s="2">
-        <v>1</v>
+        <v>19800</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>106</v>
+        <v>126</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>115</v>
+        <v>173</v>
       </c>
       <c r="E37" s="3">
         <v>2023</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>96</v>
+        <v>51</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>96</v>
+        <v>51</v>
       </c>
       <c r="H37" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="E38" s="3">
         <v>2023</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="H38" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="E39" s="3">
         <v>2023</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="H39" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>159</v>
+        <v>174</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="E40" s="3">
         <v>2023</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="H40" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>160</v>
+        <v>175</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="E41" s="3">
         <v>2023</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="H41" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>161</v>
+        <v>176</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="E42" s="3">
         <v>2023</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="H42" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>162</v>
+        <v>177</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="E43" s="3">
         <v>2023</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="H43" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="1"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="1"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="1"/>
+    <row r="44" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E44" s="3">
+        <v>2023</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H44" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E45" s="3">
+        <v>2023</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H45" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E46" s="3">
+        <v>2023</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H46" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B47" s="1"/>
+      <c r="A47" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2">
+        <v>2023</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="H47" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
@@ -2190,9 +2286,18 @@
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" s="1"/>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B71" s="1"/>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B72" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;R_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Official Use Only</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>